<commit_message>
js -> ts: mjs for node build files
Former-commit-id: c47369aa5d72733731b9444f5ec126e3a4a2a500
</commit_message>
<xml_diff>
--- a/lib/gen-server/port-battle.xlsx
+++ b/lib/gen-server/port-battle.xlsx
@@ -50,135 +50,135 @@
     <t>2. Enter player names</t>
   </si>
   <si>
+    <t>L’Océan</t>
+  </si>
+  <si>
+    <t>Santísima Trinidad</t>
+  </si>
+  <si>
+    <t>Victory</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Le Bucentaure</t>
+  </si>
+  <si>
+    <t>St. Pavel</t>
+  </si>
+  <si>
+    <t>Admiraal de Ruyter</t>
+  </si>
+  <si>
+    <t>Implacable</t>
+  </si>
+  <si>
+    <t>Redoutable</t>
+  </si>
+  <si>
+    <t>Bellona</t>
+  </si>
+  <si>
+    <t>3rd Rate</t>
+  </si>
+  <si>
+    <t>Constitution</t>
+  </si>
+  <si>
+    <t>USS United States</t>
+  </si>
+  <si>
+    <t>Wasa</t>
+  </si>
+  <si>
+    <t>Agamemnon</t>
+  </si>
+  <si>
+    <t>Rättvisan</t>
+  </si>
+  <si>
+    <t>Leopard</t>
+  </si>
+  <si>
+    <t>Indefatigable</t>
+  </si>
+  <si>
+    <t>Ingermanland</t>
+  </si>
+  <si>
+    <t>Wapen von Hamburg</t>
+  </si>
+  <si>
+    <t>Endymion</t>
+  </si>
+  <si>
+    <t>Trincomalee</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>L’Hermione</t>
+  </si>
+  <si>
+    <t>Essex</t>
+  </si>
+  <si>
+    <t>Santa Cecilia</t>
+  </si>
+  <si>
     <t>La Belle-Poule</t>
   </si>
   <si>
-    <t>Bellona</t>
+    <t>Pirate Frigate</t>
+  </si>
+  <si>
+    <t>Frigate</t>
+  </si>
+  <si>
+    <t>Hulk Indiaman</t>
+  </si>
+  <si>
+    <t>Le Gros Ventre Refit</t>
+  </si>
+  <si>
+    <t>Indiaman</t>
+  </si>
+  <si>
+    <t>La Renommée</t>
+  </si>
+  <si>
+    <t>Le Gros Ventre</t>
+  </si>
+  <si>
+    <t>Surprise</t>
+  </si>
+  <si>
+    <t>Hercules</t>
+  </si>
+  <si>
+    <t>Cerberus</t>
+  </si>
+  <si>
+    <t>Pandora</t>
+  </si>
+  <si>
+    <t>Tutorial Cerberus</t>
+  </si>
+  <si>
+    <t>Niagara</t>
   </si>
   <si>
     <t>Mortar Brig</t>
   </si>
   <si>
-    <t>Le Bucentaure</t>
-  </si>
-  <si>
-    <t>Cerberus</t>
-  </si>
-  <si>
-    <t>USS United States</t>
-  </si>
-  <si>
-    <t>Essex</t>
-  </si>
-  <si>
-    <t>Frigate</t>
-  </si>
-  <si>
-    <t>Niagara</t>
-  </si>
-  <si>
-    <t>St. Pavel</t>
-  </si>
-  <si>
-    <t>Pirate Frigate</t>
+    <t>Le Requin</t>
   </si>
   <si>
     <t>Rattlesnake Heavy</t>
   </si>
   <si>
-    <t>La Renommée</t>
-  </si>
-  <si>
-    <t>Santísima Trinidad</t>
-  </si>
-  <si>
-    <t>Surprise</t>
-  </si>
-  <si>
-    <t>Trincomalee</t>
-  </si>
-  <si>
-    <t>Victory</t>
-  </si>
-  <si>
-    <t>3rd Rate</t>
-  </si>
-  <si>
-    <t>Ingermanland</t>
-  </si>
-  <si>
-    <t>Le Gros Ventre</t>
-  </si>
-  <si>
-    <t>Indiaman</t>
-  </si>
-  <si>
-    <t>Santa Cecilia</t>
-  </si>
-  <si>
-    <t>L’Océan</t>
-  </si>
-  <si>
-    <t>Agamemnon</t>
-  </si>
-  <si>
-    <t>Endymion</t>
-  </si>
-  <si>
-    <t>Indefatigable</t>
-  </si>
-  <si>
-    <t>Wapen von Hamburg</t>
-  </si>
-  <si>
-    <t>L’Hermione</t>
-  </si>
-  <si>
-    <t>Pandora</t>
-  </si>
-  <si>
-    <t>Wasa</t>
-  </si>
-  <si>
-    <t>Le Gros Ventre Refit</t>
-  </si>
-  <si>
-    <t>Christian</t>
-  </si>
-  <si>
-    <t>Diana</t>
-  </si>
-  <si>
-    <t>Constitution</t>
-  </si>
-  <si>
-    <t>Hercules</t>
-  </si>
-  <si>
-    <t>Le Requin</t>
-  </si>
-  <si>
-    <t>Rättvisan</t>
-  </si>
-  <si>
-    <t>Leopard</t>
-  </si>
-  <si>
-    <t>Hulk Indiaman</t>
-  </si>
-  <si>
-    <t>Redoutable</t>
-  </si>
-  <si>
-    <t>Implacable</t>
-  </si>
-  <si>
-    <t>Admiraal de Ruyter</t>
-  </si>
-  <si>
-    <t>Tutorial Cerberus</t>
-  </si>
-  <si>
     <t>Aguadilla</t>
   </si>
   <si>
@@ -1109,49 +1109,49 @@
     <t>X</t>
   </si>
   <si>
+    <t>Prince de Neufchâtel</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>Navy Brig</t>
+  </si>
+  <si>
+    <t>Rattlesnake</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
     <t>Brig</t>
   </si>
   <si>
+    <t>Tutorial Trader</t>
+  </si>
+  <si>
+    <t>Tutorial Brig</t>
+  </si>
+  <si>
+    <t>Pickle</t>
+  </si>
+  <si>
     <t>Cutter</t>
   </si>
   <si>
+    <t>GunBoat</t>
+  </si>
+  <si>
+    <t>Privateer</t>
+  </si>
+  <si>
+    <t>Yacht</t>
+  </si>
+  <si>
+    <t>Yacht Silver</t>
+  </si>
+  <si>
     <t>Lynx</t>
-  </si>
-  <si>
-    <t>Mercury</t>
-  </si>
-  <si>
-    <t>Navy Brig</t>
-  </si>
-  <si>
-    <t>Pickle</t>
-  </si>
-  <si>
-    <t>Privateer</t>
-  </si>
-  <si>
-    <t>Rattlesnake</t>
-  </si>
-  <si>
-    <t>Snow</t>
-  </si>
-  <si>
-    <t>Yacht</t>
-  </si>
-  <si>
-    <t>Yacht Silver</t>
-  </si>
-  <si>
-    <t>GunBoat</t>
-  </si>
-  <si>
-    <t>Prince de Neufchâtel</t>
-  </si>
-  <si>
-    <t>Tutorial Brig</t>
-  </si>
-  <si>
-    <t>Tutorial Trader</t>
   </si>
   <si>
     <t>Ahumada</t>
@@ -1800,13 +1800,13 @@
     </row>
     <row r="5" spans="1:32" customHeight="1">
       <c r="A5" s="26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="26" t="n">
-        <v>180</v>
+        <v>900</v>
       </c>
       <c r="D5" s="26">
         <f>COUNTA(F5:AD5)</f>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="6" spans="1:32" customHeight="1">
       <c r="A6" s="26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="26" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="D6" s="26">
         <f>COUNTA(F6:AD6)</f>
@@ -1907,46 +1907,46 @@
       </c>
     </row>
     <row r="7" spans="1:32" customHeight="1">
-      <c r="A7" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="29" t="s">
+      <c r="A7" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="30" t="n">
-        <v>80</v>
-      </c>
-      <c r="D7" s="30">
+      <c r="C7" s="26" t="n">
+        <v>800</v>
+      </c>
+      <c r="D7" s="26">
         <f>COUNTA(F7:AD7)</f>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="26">
         <f>C7*D7</f>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
-      <c r="AD7" s="29"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
       <c r="AE7" s="0" t="s">
         <v>61</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="30" t="n">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="D8" s="30">
         <f>COUNTA(F8:AD8)</f>
@@ -2003,46 +2003,46 @@
       </c>
     </row>
     <row r="9" spans="1:32" customHeight="1">
-      <c r="A9" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="26" t="n">
-        <v>100</v>
-      </c>
-      <c r="D9" s="26">
+      <c r="C9" s="30" t="n">
+        <v>550</v>
+      </c>
+      <c r="D9" s="30">
         <f>COUNTA(F9:AD9)</f>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="30">
         <f>C9*D9</f>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="28"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="29"/>
       <c r="AE9" s="0" t="s">
         <v>63</v>
       </c>
@@ -2051,46 +2051,46 @@
       </c>
     </row>
     <row r="10" spans="1:32" customHeight="1">
-      <c r="A10" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B10" s="25" t="s">
+      <c r="A10" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="26" t="n">
-        <v>400</v>
-      </c>
-      <c r="D10" s="26">
+      <c r="C10" s="30" t="n">
+        <v>540</v>
+      </c>
+      <c r="D10" s="30">
         <f>COUNTA(F10:AD10)</f>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="30">
         <f>C10*D10</f>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="28"/>
-      <c r="AA10" s="28"/>
-      <c r="AB10" s="28"/>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
       <c r="AE10" s="0" t="s">
         <v>64</v>
       </c>
@@ -2100,13 +2100,13 @@
     </row>
     <row r="11" spans="1:32" customHeight="1">
       <c r="A11" s="26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="26" t="n">
-        <v>200</v>
+        <v>550</v>
       </c>
       <c r="D11" s="26">
         <f>COUNTA(F11:AD11)</f>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="12" spans="1:32" customHeight="1">
       <c r="A12" s="26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="26" t="n">
-        <v>160</v>
+        <v>550</v>
       </c>
       <c r="D12" s="26">
         <f>COUNTA(F12:AD12)</f>
@@ -2195,46 +2195,46 @@
       </c>
     </row>
     <row r="13" spans="1:32" customHeight="1">
-      <c r="A13" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="30" t="n">
-        <v>90</v>
-      </c>
-      <c r="D13" s="30">
+      <c r="C13" s="26" t="n">
+        <v>550</v>
+      </c>
+      <c r="D13" s="26">
         <f>COUNTA(F13:AD13)</f>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="26">
         <f>C13*D13</f>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="29"/>
-      <c r="AA13" s="29"/>
-      <c r="AB13" s="29"/>
-      <c r="AC13" s="29"/>
-      <c r="AD13" s="29"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
       <c r="AE13" s="0" t="s">
         <v>67</v>
       </c>
@@ -2243,46 +2243,46 @@
       </c>
     </row>
     <row r="14" spans="1:32" customHeight="1">
-      <c r="A14" s="30" t="n">
-        <v>2</v>
-      </c>
-      <c r="B14" s="29" t="s">
+      <c r="A14" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="30" t="n">
-        <v>540</v>
-      </c>
-      <c r="D14" s="30">
+      <c r="C14" s="26" t="n">
+        <v>500</v>
+      </c>
+      <c r="D14" s="26">
         <f>COUNTA(F14:AD14)</f>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="26">
         <f>C14*D14</f>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="29"/>
-      <c r="W14" s="29"/>
-      <c r="X14" s="29"/>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="29"/>
-      <c r="AA14" s="29"/>
-      <c r="AB14" s="29"/>
-      <c r="AC14" s="29"/>
-      <c r="AD14" s="29"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="28"/>
+      <c r="AD14" s="28"/>
       <c r="AE14" s="0" t="s">
         <v>68</v>
       </c>
@@ -2292,13 +2292,13 @@
     </row>
     <row r="15" spans="1:32" customHeight="1">
       <c r="A15" s="26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="26" t="n">
-        <v>180</v>
+        <v>490</v>
       </c>
       <c r="D15" s="26">
         <f>COUNTA(F15:AD15)</f>
@@ -2339,46 +2339,46 @@
       </c>
     </row>
     <row r="16" spans="1:32" customHeight="1">
-      <c r="A16" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="30" t="n">
-        <v>100</v>
-      </c>
-      <c r="D16" s="30">
+      <c r="C16" s="26" t="n">
+        <v>400</v>
+      </c>
+      <c r="D16" s="26">
         <f>COUNTA(F16:AD16)</f>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="26">
         <f>C16*D16</f>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="29"/>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="29"/>
-      <c r="AA16" s="29"/>
-      <c r="AB16" s="29"/>
-      <c r="AC16" s="29"/>
-      <c r="AD16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="28"/>
       <c r="AE16" s="0" t="s">
         <v>70</v>
       </c>
@@ -2388,13 +2388,13 @@
     </row>
     <row r="17" spans="1:32" customHeight="1">
       <c r="A17" s="26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="26" t="n">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="D17" s="26">
         <f>COUNTA(F17:AD17)</f>
@@ -2436,13 +2436,13 @@
     </row>
     <row r="18" spans="1:32" customHeight="1">
       <c r="A18" s="26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="26" t="n">
-        <v>900</v>
+        <v>400</v>
       </c>
       <c r="D18" s="26">
         <f>COUNTA(F18:AD18)</f>
@@ -2483,46 +2483,46 @@
       </c>
     </row>
     <row r="19" spans="1:32" customHeight="1">
-      <c r="A19" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B19" s="25" t="s">
+      <c r="A19" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="26" t="n">
-        <v>120</v>
-      </c>
-      <c r="D19" s="26">
+      <c r="C19" s="30" t="n">
+        <v>340</v>
+      </c>
+      <c r="D19" s="30">
         <f>COUNTA(F19:AD19)</f>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="30">
         <f>C19*D19</f>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="29"/>
+      <c r="AC19" s="29"/>
+      <c r="AD19" s="29"/>
       <c r="AE19" s="0" t="s">
         <v>73</v>
       </c>
@@ -2531,46 +2531,46 @@
       </c>
     </row>
     <row r="20" spans="1:32" customHeight="1">
-      <c r="A20" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="25" t="s">
+      <c r="A20" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="26" t="n">
-        <v>260</v>
-      </c>
-      <c r="D20" s="26">
+      <c r="C20" s="30" t="n">
+        <v>340</v>
+      </c>
+      <c r="D20" s="30">
         <f>COUNTA(F20:AD20)</f>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="30">
         <f>C20*D20</f>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="28"/>
-      <c r="Z20" s="28"/>
-      <c r="AA20" s="28"/>
-      <c r="AB20" s="28"/>
-      <c r="AC20" s="28"/>
-      <c r="AD20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="29"/>
+      <c r="AB20" s="29"/>
+      <c r="AC20" s="29"/>
+      <c r="AD20" s="29"/>
       <c r="AE20" s="0" t="s">
         <v>74</v>
       </c>
@@ -2579,46 +2579,46 @@
       </c>
     </row>
     <row r="21" spans="1:32" customHeight="1">
-      <c r="A21" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="B21" s="25" t="s">
+      <c r="A21" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="B21" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="26" t="n">
-        <v>800</v>
-      </c>
-      <c r="D21" s="26">
+      <c r="C21" s="30" t="n">
+        <v>330</v>
+      </c>
+      <c r="D21" s="30">
         <f>COUNTA(F21:AD21)</f>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="30">
         <f>C21*D21</f>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="28"/>
-      <c r="V21" s="28"/>
-      <c r="W21" s="28"/>
-      <c r="X21" s="28"/>
-      <c r="Y21" s="28"/>
-      <c r="Z21" s="28"/>
-      <c r="AA21" s="28"/>
-      <c r="AB21" s="28"/>
-      <c r="AC21" s="28"/>
-      <c r="AD21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
       <c r="AE21" s="0" t="s">
         <v>75</v>
       </c>
@@ -2627,46 +2627,46 @@
       </c>
     </row>
     <row r="22" spans="1:32" customHeight="1">
-      <c r="A22" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="25" t="s">
+      <c r="A22" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="26" t="n">
-        <v>490</v>
-      </c>
-      <c r="D22" s="26">
+      <c r="C22" s="30" t="n">
+        <v>320</v>
+      </c>
+      <c r="D22" s="30">
         <f>COUNTA(F22:AD22)</f>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="30">
         <f>C22*D22</f>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="29"/>
+      <c r="AD22" s="29"/>
       <c r="AE22" s="0" t="s">
         <v>76</v>
       </c>
@@ -2723,46 +2723,46 @@
       </c>
     </row>
     <row r="24" spans="1:32" customHeight="1">
-      <c r="A24" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B24" s="25" t="s">
+      <c r="A24" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="26" t="n">
-        <v>120</v>
-      </c>
-      <c r="D24" s="26">
+      <c r="C24" s="30" t="n">
+        <v>290</v>
+      </c>
+      <c r="D24" s="30">
         <f>COUNTA(F24:AD24)</f>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="30">
         <f>C24*D24</f>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="28"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="28"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="28"/>
-      <c r="AD24" s="28"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
+      <c r="AA24" s="29"/>
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="29"/>
+      <c r="AD24" s="29"/>
       <c r="AE24" s="0" t="s">
         <v>78</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="26" t="n">
-        <v>140</v>
+        <v>270</v>
       </c>
       <c r="D25" s="26">
         <f>COUNTA(F25:AD25)</f>
@@ -2826,7 +2826,7 @@
         <v>33</v>
       </c>
       <c r="C26" s="26" t="n">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="D26" s="26">
         <f>COUNTA(F26:AD26)</f>
@@ -2868,13 +2868,13 @@
     </row>
     <row r="27" spans="1:32" customHeight="1">
       <c r="A27" s="26" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="26" t="n">
-        <v>900</v>
+        <v>250</v>
       </c>
       <c r="D27" s="26">
         <f>COUNTA(F27:AD27)</f>
@@ -2915,46 +2915,46 @@
       </c>
     </row>
     <row r="28" spans="1:32" customHeight="1">
-      <c r="A28" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="B28" s="29" t="s">
+      <c r="A28" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="30" t="n">
-        <v>340</v>
-      </c>
-      <c r="D28" s="30">
+      <c r="C28" s="26" t="n">
+        <v>215</v>
+      </c>
+      <c r="D28" s="26">
         <f>COUNTA(F28:AD28)</f>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="26">
         <f>C28*D28</f>
       </c>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
-      <c r="U28" s="29"/>
-      <c r="V28" s="29"/>
-      <c r="W28" s="29"/>
-      <c r="X28" s="29"/>
-      <c r="Y28" s="29"/>
-      <c r="Z28" s="29"/>
-      <c r="AA28" s="29"/>
-      <c r="AB28" s="29"/>
-      <c r="AC28" s="29"/>
-      <c r="AD28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="28"/>
+      <c r="V28" s="28"/>
+      <c r="W28" s="28"/>
+      <c r="X28" s="28"/>
+      <c r="Y28" s="28"/>
+      <c r="Z28" s="28"/>
+      <c r="AA28" s="28"/>
+      <c r="AB28" s="28"/>
+      <c r="AC28" s="28"/>
+      <c r="AD28" s="28"/>
       <c r="AE28" s="0" t="s">
         <v>82</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>36</v>
       </c>
       <c r="C29" s="26" t="n">
-        <v>270</v>
+        <v>200</v>
       </c>
       <c r="D29" s="26">
         <f>COUNTA(F29:AD29)</f>
@@ -3011,46 +3011,46 @@
       </c>
     </row>
     <row r="30" spans="1:32" customHeight="1">
-      <c r="A30" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="B30" s="29" t="s">
+      <c r="A30" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="30" t="n">
-        <v>320</v>
-      </c>
-      <c r="D30" s="30">
+      <c r="C30" s="26" t="n">
+        <v>200</v>
+      </c>
+      <c r="D30" s="26">
         <f>COUNTA(F30:AD30)</f>
       </c>
-      <c r="E30" s="30">
+      <c r="E30" s="26">
         <f>C30*D30</f>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="29"/>
-      <c r="U30" s="29"/>
-      <c r="V30" s="29"/>
-      <c r="W30" s="29"/>
-      <c r="X30" s="29"/>
-      <c r="Y30" s="29"/>
-      <c r="Z30" s="29"/>
-      <c r="AA30" s="29"/>
-      <c r="AB30" s="29"/>
-      <c r="AC30" s="29"/>
-      <c r="AD30" s="29"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="28"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="28"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="28"/>
+      <c r="AD30" s="28"/>
       <c r="AE30" s="0" t="s">
         <v>84</v>
       </c>
@@ -3059,46 +3059,46 @@
       </c>
     </row>
     <row r="31" spans="1:32" customHeight="1">
-      <c r="A31" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="B31" s="29" t="s">
+      <c r="A31" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="30" t="n">
-        <v>290</v>
-      </c>
-      <c r="D31" s="30">
+      <c r="C31" s="26" t="n">
+        <v>180</v>
+      </c>
+      <c r="D31" s="26">
         <f>COUNTA(F31:AD31)</f>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="26">
         <f>C31*D31</f>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="29"/>
-      <c r="T31" s="29"/>
-      <c r="U31" s="29"/>
-      <c r="V31" s="29"/>
-      <c r="W31" s="29"/>
-      <c r="X31" s="29"/>
-      <c r="Y31" s="29"/>
-      <c r="Z31" s="29"/>
-      <c r="AA31" s="29"/>
-      <c r="AB31" s="29"/>
-      <c r="AC31" s="29"/>
-      <c r="AD31" s="29"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+      <c r="U31" s="28"/>
+      <c r="V31" s="28"/>
+      <c r="W31" s="28"/>
+      <c r="X31" s="28"/>
+      <c r="Y31" s="28"/>
+      <c r="Z31" s="28"/>
+      <c r="AA31" s="28"/>
+      <c r="AB31" s="28"/>
+      <c r="AC31" s="28"/>
+      <c r="AD31" s="28"/>
       <c r="AE31" s="0" t="s">
         <v>85</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="26" t="n">
-        <v>215</v>
+        <v>180</v>
       </c>
       <c r="D32" s="26">
         <f>COUNTA(F32:AD32)</f>
@@ -3162,7 +3162,7 @@
         <v>40</v>
       </c>
       <c r="C33" s="26" t="n">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="D33" s="26">
         <f>COUNTA(F33:AD33)</f>
@@ -3204,13 +3204,13 @@
     </row>
     <row r="34" spans="1:32" customHeight="1">
       <c r="A34" s="26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="26" t="n">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="D34" s="26">
         <f>COUNTA(F34:AD34)</f>
@@ -3299,46 +3299,46 @@
       </c>
     </row>
     <row r="36" spans="1:32" customHeight="1">
-      <c r="A36" s="30" t="n">
-        <v>2</v>
-      </c>
-      <c r="B36" s="29" t="s">
+      <c r="A36" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="30" t="n">
-        <v>600</v>
-      </c>
-      <c r="D36" s="30">
+      <c r="C36" s="26" t="n">
+        <v>140</v>
+      </c>
+      <c r="D36" s="26">
         <f>COUNTA(F36:AD36)</f>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="26">
         <f>C36*D36</f>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="29"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="29"/>
-      <c r="X36" s="29"/>
-      <c r="Y36" s="29"/>
-      <c r="Z36" s="29"/>
-      <c r="AA36" s="29"/>
-      <c r="AB36" s="29"/>
-      <c r="AC36" s="29"/>
-      <c r="AD36" s="29"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="28"/>
+      <c r="V36" s="28"/>
+      <c r="W36" s="28"/>
+      <c r="X36" s="28"/>
+      <c r="Y36" s="28"/>
+      <c r="Z36" s="28"/>
+      <c r="AA36" s="28"/>
+      <c r="AB36" s="28"/>
+      <c r="AC36" s="28"/>
+      <c r="AD36" s="28"/>
       <c r="AE36" s="0" t="s">
         <v>90</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>44</v>
       </c>
       <c r="C37" s="26" t="n">
-        <v>250</v>
+        <v>120</v>
       </c>
       <c r="D37" s="26">
         <f>COUNTA(F37:AD37)</f>
@@ -3396,13 +3396,13 @@
     </row>
     <row r="38" spans="1:32" customHeight="1">
       <c r="A38" s="26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B38" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="26" t="n">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="D38" s="26">
         <f>COUNTA(F38:AD38)</f>
@@ -3450,7 +3450,7 @@
         <v>46</v>
       </c>
       <c r="C39" s="26" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D39" s="26">
         <f>COUNTA(F39:AD39)</f>
@@ -3491,46 +3491,46 @@
       </c>
     </row>
     <row r="40" spans="1:32" customHeight="1">
-      <c r="A40" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B40" s="29" t="s">
+      <c r="A40" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="30" t="n">
-        <v>100</v>
-      </c>
-      <c r="D40" s="30">
+      <c r="C40" s="26" t="n">
+        <v>110</v>
+      </c>
+      <c r="D40" s="26">
         <f>COUNTA(F40:AD40)</f>
       </c>
-      <c r="E40" s="30">
+      <c r="E40" s="26">
         <f>C40*D40</f>
       </c>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="28"/>
+      <c r="W40" s="28"/>
+      <c r="X40" s="28"/>
+      <c r="Y40" s="28"/>
+      <c r="Z40" s="28"/>
+      <c r="AA40" s="28"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="28"/>
+      <c r="AD40" s="28"/>
       <c r="AE40" s="0" t="s">
         <v>94</v>
       </c>
@@ -3539,46 +3539,46 @@
       </c>
     </row>
     <row r="41" spans="1:32" customHeight="1">
-      <c r="A41" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="B41" s="29" t="s">
+      <c r="A41" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B41" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="30" t="n">
-        <v>340</v>
-      </c>
-      <c r="D41" s="30">
+      <c r="C41" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D41" s="26">
         <f>COUNTA(F41:AD41)</f>
       </c>
-      <c r="E41" s="30">
+      <c r="E41" s="26">
         <f>C41*D41</f>
       </c>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29"/>
-      <c r="S41" s="29"/>
-      <c r="T41" s="29"/>
-      <c r="U41" s="29"/>
-      <c r="V41" s="29"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="29"/>
-      <c r="AC41" s="29"/>
-      <c r="AD41" s="29"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="28"/>
+      <c r="R41" s="28"/>
+      <c r="S41" s="28"/>
+      <c r="T41" s="28"/>
+      <c r="U41" s="28"/>
+      <c r="V41" s="28"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
       <c r="AE41" s="0" t="s">
         <v>95</v>
       </c>
@@ -3587,46 +3587,46 @@
       </c>
     </row>
     <row r="42" spans="1:32" customHeight="1">
-      <c r="A42" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="B42" s="29" t="s">
+      <c r="A42" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B42" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="30" t="n">
-        <v>330</v>
-      </c>
-      <c r="D42" s="30">
+      <c r="C42" s="26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D42" s="26">
         <f>COUNTA(F42:AD42)</f>
       </c>
-      <c r="E42" s="30">
+      <c r="E42" s="26">
         <f>C42*D42</f>
       </c>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="28"/>
+      <c r="Y42" s="28"/>
+      <c r="Z42" s="28"/>
+      <c r="AA42" s="28"/>
+      <c r="AB42" s="28"/>
+      <c r="AC42" s="28"/>
+      <c r="AD42" s="28"/>
       <c r="AE42" s="0" t="s">
         <v>96</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="26" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D43" s="26">
         <f>COUNTA(F43:AD43)</f>
@@ -3683,46 +3683,46 @@
       </c>
     </row>
     <row r="44" spans="1:32" customHeight="1">
-      <c r="A44" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B44" s="25" t="s">
+      <c r="A44" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B44" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="26" t="n">
-        <v>550</v>
-      </c>
-      <c r="D44" s="26">
+      <c r="C44" s="30" t="n">
+        <v>90</v>
+      </c>
+      <c r="D44" s="30">
         <f>COUNTA(F44:AD44)</f>
       </c>
-      <c r="E44" s="26">
+      <c r="E44" s="30">
         <f>C44*D44</f>
       </c>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="28"/>
-      <c r="P44" s="28"/>
-      <c r="Q44" s="28"/>
-      <c r="R44" s="28"/>
-      <c r="S44" s="28"/>
-      <c r="T44" s="28"/>
-      <c r="U44" s="28"/>
-      <c r="V44" s="28"/>
-      <c r="W44" s="28"/>
-      <c r="X44" s="28"/>
-      <c r="Y44" s="28"/>
-      <c r="Z44" s="28"/>
-      <c r="AA44" s="28"/>
-      <c r="AB44" s="28"/>
-      <c r="AC44" s="28"/>
-      <c r="AD44" s="28"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
       <c r="AE44" s="0" t="s">
         <v>98</v>
       </c>
@@ -3731,46 +3731,46 @@
       </c>
     </row>
     <row r="45" spans="1:32" customHeight="1">
-      <c r="A45" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B45" s="25" t="s">
+      <c r="A45" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B45" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="26" t="n">
-        <v>550</v>
-      </c>
-      <c r="D45" s="26">
+      <c r="C45" s="30" t="n">
+        <v>80</v>
+      </c>
+      <c r="D45" s="30">
         <f>COUNTA(F45:AD45)</f>
       </c>
-      <c r="E45" s="26">
+      <c r="E45" s="30">
         <f>C45*D45</f>
       </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="28"/>
-      <c r="Q45" s="28"/>
-      <c r="R45" s="28"/>
-      <c r="S45" s="28"/>
-      <c r="T45" s="28"/>
-      <c r="U45" s="28"/>
-      <c r="V45" s="28"/>
-      <c r="W45" s="28"/>
-      <c r="X45" s="28"/>
-      <c r="Y45" s="28"/>
-      <c r="Z45" s="28"/>
-      <c r="AA45" s="28"/>
-      <c r="AB45" s="28"/>
-      <c r="AC45" s="28"/>
-      <c r="AD45" s="28"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="29"/>
+      <c r="Q45" s="29"/>
+      <c r="R45" s="29"/>
+      <c r="S45" s="29"/>
+      <c r="T45" s="29"/>
+      <c r="U45" s="29"/>
+      <c r="V45" s="29"/>
+      <c r="W45" s="29"/>
+      <c r="X45" s="29"/>
+      <c r="Y45" s="29"/>
+      <c r="Z45" s="29"/>
+      <c r="AA45" s="29"/>
+      <c r="AB45" s="29"/>
+      <c r="AC45" s="29"/>
+      <c r="AD45" s="29"/>
       <c r="AE45" s="0" t="s">
         <v>99</v>
       </c>
@@ -3779,46 +3779,46 @@
       </c>
     </row>
     <row r="46" spans="1:32" customHeight="1">
-      <c r="A46" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B46" s="25" t="s">
+      <c r="A46" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B46" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="26" t="n">
-        <v>550</v>
-      </c>
-      <c r="D46" s="26">
+      <c r="C46" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D46" s="30">
         <f>COUNTA(F46:AD46)</f>
       </c>
-      <c r="E46" s="26">
+      <c r="E46" s="30">
         <f>C46*D46</f>
       </c>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="28"/>
-      <c r="P46" s="28"/>
-      <c r="Q46" s="28"/>
-      <c r="R46" s="28"/>
-      <c r="S46" s="28"/>
-      <c r="T46" s="28"/>
-      <c r="U46" s="28"/>
-      <c r="V46" s="28"/>
-      <c r="W46" s="28"/>
-      <c r="X46" s="28"/>
-      <c r="Y46" s="28"/>
-      <c r="Z46" s="28"/>
-      <c r="AA46" s="28"/>
-      <c r="AB46" s="28"/>
-      <c r="AC46" s="28"/>
-      <c r="AD46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="29"/>
+      <c r="N46" s="29"/>
+      <c r="O46" s="29"/>
+      <c r="P46" s="29"/>
+      <c r="Q46" s="29"/>
+      <c r="R46" s="29"/>
+      <c r="S46" s="29"/>
+      <c r="T46" s="29"/>
+      <c r="U46" s="29"/>
+      <c r="V46" s="29"/>
+      <c r="W46" s="29"/>
+      <c r="X46" s="29"/>
+      <c r="Y46" s="29"/>
+      <c r="Z46" s="29"/>
+      <c r="AA46" s="29"/>
+      <c r="AB46" s="29"/>
+      <c r="AC46" s="29"/>
+      <c r="AD46" s="29"/>
       <c r="AE46" s="0" t="s">
         <v>100</v>
       </c>
@@ -3827,46 +3827,46 @@
       </c>
     </row>
     <row r="47" spans="1:32" customHeight="1">
-      <c r="A47" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B47" s="25" t="s">
+      <c r="A47" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B47" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="26" t="n">
+      <c r="C47" s="30" t="n">
         <v>100</v>
       </c>
-      <c r="D47" s="26">
+      <c r="D47" s="30">
         <f>COUNTA(F47:AD47)</f>
       </c>
-      <c r="E47" s="26">
+      <c r="E47" s="30">
         <f>C47*D47</f>
       </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="28"/>
-      <c r="N47" s="28"/>
-      <c r="O47" s="28"/>
-      <c r="P47" s="28"/>
-      <c r="Q47" s="28"/>
-      <c r="R47" s="28"/>
-      <c r="S47" s="28"/>
-      <c r="T47" s="28"/>
-      <c r="U47" s="28"/>
-      <c r="V47" s="28"/>
-      <c r="W47" s="28"/>
-      <c r="X47" s="28"/>
-      <c r="Y47" s="28"/>
-      <c r="Z47" s="28"/>
-      <c r="AA47" s="28"/>
-      <c r="AB47" s="28"/>
-      <c r="AC47" s="28"/>
-      <c r="AD47" s="28"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
+      <c r="T47" s="29"/>
+      <c r="U47" s="29"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+      <c r="X47" s="29"/>
+      <c r="Y47" s="29"/>
+      <c r="Z47" s="29"/>
+      <c r="AA47" s="29"/>
+      <c r="AB47" s="29"/>
+      <c r="AC47" s="29"/>
+      <c r="AD47" s="29"/>
       <c r="AE47" s="0" t="s">
         <v>101</v>
       </c>
@@ -6150,10 +6150,10 @@
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="21">
-        <f>SUM(D5:D28)</f>
+        <f>SUM(D5:D29)</f>
       </c>
       <c r="E4" s="21">
-        <f>SUM(E5:E28)</f>
+        <f>SUM(E5:E29)</f>
       </c>
       <c r="F4" s="22" t="s">
         <v>11</v>
@@ -6190,52 +6190,52 @@
       </c>
     </row>
     <row r="5" spans="1:32" customHeight="1">
-      <c r="A5" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="C5" s="30" t="n">
-        <v>45</v>
-      </c>
-      <c r="D5" s="30">
+      <c r="A5" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="26" t="n">
+        <v>215</v>
+      </c>
+      <c r="D5" s="26">
         <f>COUNTA(F5:AD5)</f>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="26">
         <f>C5*D5</f>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>360</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
       <c r="AE5" s="0" t="s">
         <v>384</v>
       </c>
@@ -6244,52 +6244,52 @@
       </c>
     </row>
     <row r="6" spans="1:32" customHeight="1">
-      <c r="A6" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="30" t="n">
-        <v>80</v>
-      </c>
-      <c r="D6" s="30">
+      <c r="A6" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="26" t="n">
+        <v>120</v>
+      </c>
+      <c r="D6" s="26">
         <f>COUNTA(F6:AD6)</f>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="26">
         <f>C6*D6</f>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
       <c r="AE6" s="0" t="s">
         <v>385</v>
       </c>
@@ -6302,10 +6302,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C7" s="26" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D7" s="26">
         <f>COUNTA(F7:AD7)</f>
@@ -6347,13 +6347,13 @@
     </row>
     <row r="8" spans="1:32" customHeight="1">
       <c r="A8" s="26" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>366</v>
+        <v>47</v>
       </c>
       <c r="C8" s="26" t="n">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="D8" s="26">
         <f>COUNTA(F8:AD8)</f>
@@ -6395,13 +6395,13 @@
     </row>
     <row r="9" spans="1:32" customHeight="1">
       <c r="A9" s="26" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>367</v>
+        <v>48</v>
       </c>
       <c r="C9" s="26" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D9" s="26">
         <f>COUNTA(F9:AD9)</f>
@@ -6446,10 +6446,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>368</v>
+        <v>51</v>
       </c>
       <c r="C10" s="30" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D10" s="30">
         <f>COUNTA(F10:AD10)</f>
@@ -6494,10 +6494,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>369</v>
+        <v>52</v>
       </c>
       <c r="C11" s="30" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D11" s="30">
         <f>COUNTA(F11:AD11)</f>
@@ -6542,10 +6542,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>20</v>
+        <v>365</v>
       </c>
       <c r="C12" s="30" t="n">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D12" s="30">
         <f>COUNTA(F12:AD12)</f>
@@ -6586,46 +6586,46 @@
       </c>
     </row>
     <row r="13" spans="1:32" customHeight="1">
-      <c r="A13" s="26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="C13" s="26" t="n">
-        <v>35</v>
-      </c>
-      <c r="D13" s="26">
+      <c r="A13" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" s="30" t="n">
+        <v>60</v>
+      </c>
+      <c r="D13" s="30">
         <f>COUNTA(F13:AD13)</f>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="30">
         <f>C13*D13</f>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29"/>
+      <c r="AC13" s="29"/>
+      <c r="AD13" s="29"/>
       <c r="AE13" s="0" t="s">
         <v>392</v>
       </c>
@@ -6634,46 +6634,46 @@
       </c>
     </row>
     <row r="14" spans="1:32" customHeight="1">
-      <c r="A14" s="26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>371</v>
-      </c>
-      <c r="C14" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="D14" s="26">
+      <c r="A14" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="C14" s="30" t="n">
+        <v>60</v>
+      </c>
+      <c r="D14" s="30">
         <f>COUNTA(F14:AD14)</f>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="30">
         <f>C14*D14</f>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
-      <c r="W14" s="28"/>
-      <c r="X14" s="28"/>
-      <c r="Y14" s="28"/>
-      <c r="Z14" s="28"/>
-      <c r="AA14" s="28"/>
-      <c r="AB14" s="28"/>
-      <c r="AC14" s="28"/>
-      <c r="AD14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="29"/>
+      <c r="AB14" s="29"/>
+      <c r="AC14" s="29"/>
+      <c r="AD14" s="29"/>
       <c r="AE14" s="0" t="s">
         <v>393</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C15" s="30" t="n">
         <v>60</v>
@@ -6734,10 +6734,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>23</v>
+        <v>369</v>
       </c>
       <c r="C16" s="30" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D16" s="30">
         <f>COUNTA(F16:AD16)</f>
@@ -6778,46 +6778,46 @@
       </c>
     </row>
     <row r="17" spans="1:32" customHeight="1">
-      <c r="A17" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="26" t="n">
-        <v>120</v>
-      </c>
-      <c r="D17" s="26">
+      <c r="A17" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="C17" s="30" t="n">
+        <v>45</v>
+      </c>
+      <c r="D17" s="30">
         <f>COUNTA(F17:AD17)</f>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="30">
         <f>C17*D17</f>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="28"/>
-      <c r="AA17" s="28"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="28"/>
-      <c r="AD17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="29"/>
       <c r="AE17" s="0" t="s">
         <v>396</v>
       </c>
@@ -6830,10 +6830,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C18" s="30" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D18" s="30">
         <f>COUNTA(F18:AD18)</f>
@@ -6874,46 +6874,46 @@
       </c>
     </row>
     <row r="19" spans="1:32" customHeight="1">
-      <c r="A19" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="26" t="n">
-        <v>120</v>
-      </c>
-      <c r="D19" s="26">
+      <c r="A19" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="C19" s="30" t="n">
+        <v>30</v>
+      </c>
+      <c r="D19" s="30">
         <f>COUNTA(F19:AD19)</f>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="30">
         <f>C19*D19</f>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="29"/>
+      <c r="AC19" s="29"/>
+      <c r="AD19" s="29"/>
       <c r="AE19" s="0" t="s">
         <v>398</v>
       </c>
@@ -6922,46 +6922,46 @@
       </c>
     </row>
     <row r="20" spans="1:32" customHeight="1">
-      <c r="A20" s="26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>374</v>
-      </c>
-      <c r="C20" s="26" t="n">
+      <c r="A20" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="C20" s="30" t="n">
         <v>30</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="30">
         <f>COUNTA(F20:AD20)</f>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="30">
         <f>C20*D20</f>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="28"/>
-      <c r="Z20" s="28"/>
-      <c r="AA20" s="28"/>
-      <c r="AB20" s="28"/>
-      <c r="AC20" s="28"/>
-      <c r="AD20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="29"/>
+      <c r="AB20" s="29"/>
+      <c r="AC20" s="29"/>
+      <c r="AD20" s="29"/>
       <c r="AE20" s="0" t="s">
         <v>399</v>
       </c>
@@ -6970,46 +6970,46 @@
       </c>
     </row>
     <row r="21" spans="1:32" customHeight="1">
-      <c r="A21" s="26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>375</v>
-      </c>
-      <c r="C21" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="D21" s="26">
+      <c r="A21" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" s="30">
         <f>COUNTA(F21:AD21)</f>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="30">
         <f>C21*D21</f>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="28"/>
-      <c r="V21" s="28"/>
-      <c r="W21" s="28"/>
-      <c r="X21" s="28"/>
-      <c r="Y21" s="28"/>
-      <c r="Z21" s="28"/>
-      <c r="AA21" s="28"/>
-      <c r="AB21" s="28"/>
-      <c r="AC21" s="28"/>
-      <c r="AD21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
       <c r="AE21" s="0" t="s">
         <v>400</v>
       </c>
@@ -7018,46 +7018,46 @@
       </c>
     </row>
     <row r="22" spans="1:32" customHeight="1">
-      <c r="A22" s="26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="C22" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="D22" s="26">
+      <c r="A22" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" s="30">
         <f>COUNTA(F22:AD22)</f>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="30">
         <f>C22*D22</f>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="29"/>
+      <c r="AD22" s="29"/>
       <c r="AE22" s="0" t="s">
         <v>401</v>
       </c>
@@ -7067,13 +7067,13 @@
     </row>
     <row r="23" spans="1:32" customHeight="1">
       <c r="A23" s="26" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>39</v>
+        <v>373</v>
       </c>
       <c r="C23" s="26" t="n">
-        <v>215</v>
+        <v>35</v>
       </c>
       <c r="D23" s="26">
         <f>COUNTA(F23:AD23)</f>
@@ -7114,46 +7114,46 @@
       </c>
     </row>
     <row r="24" spans="1:32" customHeight="1">
-      <c r="A24" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>377</v>
-      </c>
-      <c r="C24" s="30" t="n">
-        <v>65</v>
-      </c>
-      <c r="D24" s="30">
+      <c r="A24" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="C24" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="D24" s="26">
         <f>COUNTA(F24:AD24)</f>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="26">
         <f>C24*D24</f>
       </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="29"/>
-      <c r="Q24" s="29"/>
-      <c r="R24" s="29"/>
-      <c r="S24" s="29"/>
-      <c r="T24" s="29"/>
-      <c r="U24" s="29"/>
-      <c r="V24" s="29"/>
-      <c r="W24" s="29"/>
-      <c r="X24" s="29"/>
-      <c r="Y24" s="29"/>
-      <c r="Z24" s="29"/>
-      <c r="AA24" s="29"/>
-      <c r="AB24" s="29"/>
-      <c r="AC24" s="29"/>
-      <c r="AD24" s="29"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="28"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="28"/>
+      <c r="AD24" s="28"/>
       <c r="AE24" s="0" t="s">
         <v>403</v>
       </c>
@@ -7162,46 +7162,46 @@
       </c>
     </row>
     <row r="25" spans="1:32" customHeight="1">
-      <c r="A25" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="C25" s="30" t="n">
+      <c r="A25" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="C25" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="26">
         <f>COUNTA(F25:AD25)</f>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="26">
         <f>C25*D25</f>
       </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="29"/>
-      <c r="T25" s="29"/>
-      <c r="U25" s="29"/>
-      <c r="V25" s="29"/>
-      <c r="W25" s="29"/>
-      <c r="X25" s="29"/>
-      <c r="Y25" s="29"/>
-      <c r="Z25" s="29"/>
-      <c r="AA25" s="29"/>
-      <c r="AB25" s="29"/>
-      <c r="AC25" s="29"/>
-      <c r="AD25" s="29"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="28"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="28"/>
+      <c r="X25" s="28"/>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="28"/>
+      <c r="AA25" s="28"/>
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="28"/>
+      <c r="AD25" s="28"/>
       <c r="AE25" s="0" t="s">
         <v>404</v>
       </c>
@@ -7211,13 +7211,13 @@
     </row>
     <row r="26" spans="1:32" customHeight="1">
       <c r="A26" s="26" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>46</v>
+        <v>376</v>
       </c>
       <c r="C26" s="26" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="D26" s="26">
         <f>COUNTA(F26:AD26)</f>
@@ -7258,46 +7258,46 @@
       </c>
     </row>
     <row r="27" spans="1:32" customHeight="1">
-      <c r="A27" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="30" t="n">
-        <v>100</v>
-      </c>
-      <c r="D27" s="30">
+      <c r="A27" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="C27" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="D27" s="26">
         <f>COUNTA(F27:AD27)</f>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="26">
         <f>C27*D27</f>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="29"/>
-      <c r="T27" s="29"/>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="29"/>
-      <c r="X27" s="29"/>
-      <c r="Y27" s="29"/>
-      <c r="Z27" s="29"/>
-      <c r="AA27" s="29"/>
-      <c r="AB27" s="29"/>
-      <c r="AC27" s="29"/>
-      <c r="AD27" s="29"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="28"/>
+      <c r="X27" s="28"/>
+      <c r="Y27" s="28"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="28"/>
+      <c r="AC27" s="28"/>
+      <c r="AD27" s="28"/>
       <c r="AE27" s="0" t="s">
         <v>406</v>
       </c>
@@ -7306,46 +7306,46 @@
       </c>
     </row>
     <row r="28" spans="1:32" customHeight="1">
-      <c r="A28" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>379</v>
-      </c>
-      <c r="C28" s="30" t="n">
-        <v>45</v>
-      </c>
-      <c r="D28" s="30">
+      <c r="A28" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C28" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="D28" s="26">
         <f>COUNTA(F28:AD28)</f>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="26">
         <f>C28*D28</f>
       </c>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
-      <c r="U28" s="29"/>
-      <c r="V28" s="29"/>
-      <c r="W28" s="29"/>
-      <c r="X28" s="29"/>
-      <c r="Y28" s="29"/>
-      <c r="Z28" s="29"/>
-      <c r="AA28" s="29"/>
-      <c r="AB28" s="29"/>
-      <c r="AC28" s="29"/>
-      <c r="AD28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="28"/>
+      <c r="V28" s="28"/>
+      <c r="W28" s="28"/>
+      <c r="X28" s="28"/>
+      <c r="Y28" s="28"/>
+      <c r="Z28" s="28"/>
+      <c r="AA28" s="28"/>
+      <c r="AB28" s="28"/>
+      <c r="AC28" s="28"/>
+      <c r="AD28" s="28"/>
       <c r="AE28" s="0" t="s">
         <v>407</v>
       </c>
@@ -7353,7 +7353,47 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="29" spans="31:32" customHeight="1">
+    <row r="29" spans="1:32" customHeight="1">
+      <c r="A29" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="C29" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="D29" s="26">
+        <f>COUNTA(F29:AD29)</f>
+      </c>
+      <c r="E29" s="26">
+        <f>C29*D29</f>
+      </c>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="28"/>
+      <c r="Z29" s="28"/>
+      <c r="AA29" s="28"/>
+      <c r="AB29" s="28"/>
+      <c r="AC29" s="28"/>
+      <c r="AD29" s="28"/>
       <c r="AE29" s="0" t="s">
         <v>408</v>
       </c>

</xml_diff>